<commit_message>
Cambio de libreria de xml a lxml, agregamos prefijo necesario para la validacion, modificacion de los excel
</commit_message>
<xml_diff>
--- a/DatosContrato.xlsx
+++ b/DatosContrato.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DatosViajeros\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Desktop\AutoDatosViajeros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3123FC3-BE5F-49C2-815A-80B9D85CEF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E3298BD-B626-47B2-8478-C59CE8EA8A07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{FC20CB11-AA40-4491-BB35-1EEA2A64B57E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FC20CB11-AA40-4491-BB35-1EEA2A64B57E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -195,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -212,6 +212,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,7 +566,7 @@
   <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +618,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="10">
+      <c r="A2" s="14">
         <v>123</v>
       </c>
       <c r="B2" s="11">
@@ -646,7 +648,7 @@
       <c r="J2" s="13"/>
     </row>
     <row r="3" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="7"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -660,7 +662,7 @@
       <c r="O3" s="6"/>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="15"/>
       <c r="B4" s="7"/>
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
@@ -674,7 +676,7 @@
       <c r="O4" s="6"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="15"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
@@ -688,7 +690,7 @@
       <c r="O5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="15"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
       <c r="D6" s="7"/>
@@ -702,7 +704,7 @@
       <c r="O6" s="6"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="15"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
       <c r="D7" s="7"/>
@@ -716,7 +718,7 @@
       <c r="O7" s="6"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="15"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
       <c r="D8" s="7"/>
@@ -730,7 +732,7 @@
       <c r="O8" s="6"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="15"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
       <c r="D9" s="7"/>
@@ -744,7 +746,7 @@
       <c r="O9" s="6"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="15"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -758,7 +760,7 @@
       <c r="O10" s="6"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="15"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
@@ -770,7 +772,7 @@
       <c r="J11" s="9"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="15"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
       <c r="D12" s="7"/>
@@ -782,7 +784,7 @@
       <c r="J12" s="9"/>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
@@ -794,7 +796,7 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
       <c r="D14" s="7"/>
@@ -806,7 +808,7 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -818,7 +820,7 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="15"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
       <c r="D16" s="7"/>
@@ -830,7 +832,7 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="15"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
@@ -842,7 +844,7 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="15"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
@@ -854,7 +856,7 @@
       <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="15"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
       <c r="D19" s="7"/>
@@ -866,7 +868,7 @@
       <c r="J19" s="9"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="15"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
       <c r="D20" s="7"/>
@@ -878,7 +880,7 @@
       <c r="J20" s="9"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="15"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
       <c r="D21" s="7"/>
@@ -890,7 +892,7 @@
       <c r="J21" s="9"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="15"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
       <c r="D22" s="7"/>
@@ -902,7 +904,7 @@
       <c r="J22" s="9"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
       <c r="D23" s="7"/>
@@ -914,7 +916,7 @@
       <c r="J23" s="9"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="15"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
@@ -926,7 +928,7 @@
       <c r="J24" s="9"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="15"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
       <c r="D25" s="7"/>
@@ -938,7 +940,7 @@
       <c r="J25" s="9"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="15"/>
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
@@ -950,7 +952,7 @@
       <c r="J26" s="9"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="15"/>
       <c r="B27" s="7"/>
       <c r="C27" s="7"/>
       <c r="D27" s="7"/>
@@ -962,7 +964,7 @@
       <c r="J27" s="9"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="15"/>
       <c r="B28" s="7"/>
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
@@ -974,7 +976,7 @@
       <c r="J28" s="9"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="15"/>
       <c r="B29" s="7"/>
       <c r="C29" s="7"/>
       <c r="D29" s="7"/>
@@ -986,7 +988,7 @@
       <c r="J29" s="9"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="15"/>
       <c r="B30" s="7"/>
       <c r="C30" s="7"/>
       <c r="D30" s="7"/>
@@ -998,7 +1000,7 @@
       <c r="J30" s="9"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="15"/>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
       <c r="D31" s="7"/>
@@ -1010,7 +1012,7 @@
       <c r="J31" s="9"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="15"/>
       <c r="B32" s="7"/>
       <c r="C32" s="7"/>
       <c r="D32" s="7"/>
@@ -1022,7 +1024,7 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="15"/>
       <c r="B33" s="7"/>
       <c r="C33" s="7"/>
       <c r="D33" s="7"/>
@@ -1034,7 +1036,7 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="15"/>
       <c r="B34" s="7"/>
       <c r="C34" s="7"/>
       <c r="D34" s="7"/>
@@ -1046,7 +1048,7 @@
       <c r="J34" s="9"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="15"/>
       <c r="B35" s="7"/>
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
@@ -1058,7 +1060,7 @@
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="15"/>
       <c r="B36" s="7"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
@@ -1070,7 +1072,7 @@
       <c r="J36" s="9"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="15"/>
       <c r="B37" s="7"/>
       <c r="C37" s="7"/>
       <c r="D37" s="7"/>
@@ -1082,7 +1084,7 @@
       <c r="J37" s="9"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="15"/>
       <c r="B38" s="7"/>
       <c r="C38" s="7"/>
       <c r="D38" s="7"/>
@@ -1094,7 +1096,7 @@
       <c r="J38" s="9"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="15"/>
       <c r="B39" s="7"/>
       <c r="C39" s="7"/>
       <c r="D39" s="7"/>
@@ -1106,7 +1108,7 @@
       <c r="J39" s="9"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="15"/>
       <c r="B40" s="7"/>
       <c r="C40" s="7"/>
       <c r="D40" s="7"/>
@@ -1118,7 +1120,7 @@
       <c r="J40" s="9"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="15"/>
       <c r="B41" s="7"/>
       <c r="C41" s="7"/>
       <c r="D41" s="7"/>
@@ -1130,7 +1132,7 @@
       <c r="J41" s="9"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="7"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
@@ -1142,7 +1144,7 @@
       <c r="J42" s="9"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="15"/>
       <c r="B43" s="7"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
@@ -1154,7 +1156,7 @@
       <c r="J43" s="9"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+      <c r="A44" s="15"/>
       <c r="B44" s="7"/>
       <c r="C44" s="7"/>
       <c r="D44" s="7"/>
@@ -1166,7 +1168,7 @@
       <c r="J44" s="9"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="15"/>
       <c r="B45" s="7"/>
       <c r="C45" s="7"/>
       <c r="D45" s="7"/>
@@ -1178,7 +1180,7 @@
       <c r="J45" s="9"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+      <c r="A46" s="15"/>
       <c r="B46" s="7"/>
       <c r="C46" s="7"/>
       <c r="D46" s="7"/>
@@ -1190,7 +1192,7 @@
       <c r="J46" s="9"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="15"/>
       <c r="B47" s="7"/>
       <c r="C47" s="7"/>
       <c r="D47" s="7"/>
@@ -1202,7 +1204,7 @@
       <c r="J47" s="9"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+      <c r="A48" s="15"/>
       <c r="B48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
@@ -1214,7 +1216,7 @@
       <c r="J48" s="9"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="15"/>
       <c r="B49" s="7"/>
       <c r="C49" s="7"/>
       <c r="D49" s="7"/>
@@ -1226,7 +1228,7 @@
       <c r="J49" s="9"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="15"/>
       <c r="B50" s="7"/>
       <c r="C50" s="7"/>
       <c r="D50" s="7"/>
@@ -1238,7 +1240,7 @@
       <c r="J50" s="9"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="15"/>
       <c r="B51" s="7"/>
       <c r="C51" s="7"/>
       <c r="D51" s="7"/>
@@ -1250,7 +1252,7 @@
       <c r="J51" s="9"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="15"/>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
       <c r="D52" s="7"/>
@@ -1262,7 +1264,7 @@
       <c r="J52" s="9"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+      <c r="A53" s="15"/>
       <c r="B53" s="7"/>
       <c r="C53" s="7"/>
       <c r="D53" s="7"/>

</xml_diff>